<commit_message>
added background to annotated_csv
</commit_message>
<xml_diff>
--- a/data/champion_list_master_dataset.xlsx
+++ b/data/champion_list_master_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgw/Desktop/CS686_Project/teamfight-tactics-ai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09DBF84-69D1-264B-8708-C15712791ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369FAC9E-9691-0947-B85C-5C928C06A585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="129">
   <si>
-    <t>champion</t>
-  </si>
-  <si>
     <t>origin_1</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>cost</t>
   </si>
   <si>
-    <t>Set</t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
@@ -407,6 +401,12 @@
   </si>
   <si>
     <t>Target Dummy</t>
+  </si>
+  <si>
+    <t>champion_name</t>
+  </si>
+  <si>
+    <t>set</t>
   </si>
 </sst>
 </file>
@@ -671,48 +671,48 @@
   </sheetPr>
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -723,14 +723,14 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -741,14 +741,14 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -759,14 +759,14 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -777,14 +777,14 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -795,14 +795,14 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -813,13 +813,13 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -830,30 +830,30 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -864,13 +864,13 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -898,13 +898,13 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -915,16 +915,16 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -935,13 +935,13 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G15" s="1">
         <v>2</v>
@@ -952,30 +952,30 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G16" s="1">
         <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G17" s="1">
         <v>2</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G18" s="1">
         <v>2</v>
@@ -1003,13 +1003,13 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G19" s="1">
         <v>2</v>
@@ -1020,16 +1020,16 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G20" s="1">
         <v>2</v>
@@ -1040,16 +1040,16 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G21" s="1">
         <v>2</v>
@@ -1060,30 +1060,30 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G22" s="1">
         <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G23" s="1">
         <v>2</v>
@@ -1094,30 +1094,30 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G24" s="1">
         <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G25" s="1">
         <v>2</v>
@@ -1128,13 +1128,13 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
@@ -1145,13 +1145,13 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G27" s="1">
         <v>2</v>
@@ -1162,16 +1162,16 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G28" s="1">
         <v>3</v>
@@ -1182,33 +1182,33 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G29" s="1">
         <v>3</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G30" s="1">
         <v>3</v>
@@ -1219,16 +1219,16 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G31" s="1">
         <v>3</v>
@@ -1239,30 +1239,30 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G32" s="1">
         <v>3</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G33" s="1">
         <v>3</v>
@@ -1273,13 +1273,13 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G34" s="1">
         <v>3</v>
@@ -1290,13 +1290,13 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G35" s="1">
         <v>3</v>
@@ -1307,13 +1307,13 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G36" s="1">
         <v>3</v>
@@ -1324,13 +1324,13 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G37" s="1">
         <v>3</v>
@@ -1341,13 +1341,13 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G38" s="1">
         <v>3</v>
@@ -1358,13 +1358,13 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G39" s="1">
         <v>3</v>
@@ -1375,13 +1375,13 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G40" s="1">
         <v>3</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G41" s="1">
         <v>4</v>
@@ -1409,13 +1409,13 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G42" s="1">
         <v>4</v>
@@ -1426,13 +1426,13 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G43" s="1">
         <v>4</v>
@@ -1443,13 +1443,13 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G44" s="1">
         <v>4</v>
@@ -1460,13 +1460,13 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G45" s="1">
         <v>4</v>
@@ -1477,13 +1477,13 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G46" s="1">
         <v>4</v>
@@ -1494,13 +1494,13 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G47" s="1">
         <v>4</v>
@@ -1511,13 +1511,13 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G48" s="1">
         <v>4</v>
@@ -1528,13 +1528,13 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G49" s="1">
         <v>4</v>
@@ -1545,13 +1545,13 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G50" s="1">
         <v>4</v>
@@ -1562,13 +1562,13 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G51" s="1">
         <v>4</v>
@@ -1579,36 +1579,36 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G52" s="1">
         <v>4</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G53" s="1">
         <v>5</v>
@@ -1619,16 +1619,16 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G54" s="1">
         <v>5</v>
@@ -1639,33 +1639,33 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G55" s="1">
         <v>5</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G56" s="1">
         <v>5</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G57" s="1">
         <v>5</v>
@@ -1693,16 +1693,16 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G58" s="1">
         <v>5</v>
@@ -1713,10 +1713,10 @@
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G59" s="1">
         <v>5</v>
@@ -1727,13 +1727,13 @@
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G60" s="1">
         <v>5</v>
@@ -1744,13 +1744,13 @@
     </row>
     <row r="61" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G61" s="1">
         <v>5</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="62" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H62" s="1">
         <v>6.5</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="63" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H63" s="1">
         <v>6.5</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="64" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H64" s="1">
         <v>6.5</v>
@@ -1785,13 +1785,13 @@
     </row>
     <row r="65" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H65" s="1">
         <v>6</v>
@@ -1799,13 +1799,13 @@
     </row>
     <row r="66" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H66" s="1">
         <v>6</v>
@@ -1813,13 +1813,13 @@
     </row>
     <row r="67" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="H67" s="1">
         <v>6</v>
@@ -1827,13 +1827,13 @@
     </row>
     <row r="68" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H68" s="1">
         <v>6</v>
@@ -1841,16 +1841,16 @@
     </row>
     <row r="69" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H69" s="1">
         <v>6</v>
@@ -1858,13 +1858,13 @@
     </row>
     <row r="70" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H70" s="1">
         <v>6</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="71" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H71" s="1">
         <v>6</v>
@@ -1886,16 +1886,16 @@
     </row>
     <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H72" s="1">
         <v>6</v>
@@ -1903,13 +1903,13 @@
     </row>
     <row r="73" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H73" s="1">
         <v>6</v>
@@ -1917,13 +1917,13 @@
     </row>
     <row r="74" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H74" s="1">
         <v>6</v>
@@ -1931,13 +1931,13 @@
     </row>
     <row r="75" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H75" s="1">
         <v>6</v>
@@ -1945,13 +1945,13 @@
     </row>
     <row r="76" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H76" s="1">
         <v>6</v>
@@ -1959,16 +1959,16 @@
     </row>
     <row r="77" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H77" s="1">
         <v>6</v>
@@ -1976,16 +1976,16 @@
     </row>
     <row r="78" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H78" s="1">
         <v>6</v>
@@ -1993,13 +1993,13 @@
     </row>
     <row r="79" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H79" s="1">
         <v>6</v>
@@ -2007,13 +2007,13 @@
     </row>
     <row r="80" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H80" s="1">
         <v>6</v>
@@ -2021,16 +2021,16 @@
     </row>
     <row r="81" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H81" s="1">
         <v>6</v>
@@ -2038,13 +2038,13 @@
     </row>
     <row r="82" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H82" s="1">
         <v>6</v>
@@ -2052,13 +2052,13 @@
     </row>
     <row r="83" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H83" s="1">
         <v>6</v>
@@ -2066,13 +2066,13 @@
     </row>
     <row r="84" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H84" s="1">
         <v>6</v>
@@ -2080,16 +2080,16 @@
     </row>
     <row r="85" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H85" s="1">
         <v>6</v>
@@ -2097,10 +2097,10 @@
     </row>
     <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the champion_list to include costs for missing values
</commit_message>
<xml_diff>
--- a/data/champion_list_master_dataset.xlsx
+++ b/data/champion_list_master_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgw/Desktop/CS686_Project/teamfight-tactics-ai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369FAC9E-9691-0947-B85C-5C928C06A585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38129A8D-61C1-4043-A813-E5D964FEBC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="130">
   <si>
     <t>origin_1</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>set</t>
+  </si>
+  <si>
+    <t>Bots</t>
   </si>
 </sst>
 </file>
@@ -671,8 +674,8 @@
   </sheetPr>
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1763,6 +1766,12 @@
       <c r="A62" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="B62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
       <c r="H62" s="1">
         <v>6.5</v>
       </c>
@@ -1771,6 +1780,12 @@
       <c r="A63" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="B63" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
       <c r="H63" s="1">
         <v>6.5</v>
       </c>
@@ -1779,6 +1794,12 @@
       <c r="A64" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="B64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
       <c r="H64" s="1">
         <v>6.5</v>
       </c>
@@ -1793,6 +1814,9 @@
       <c r="E65" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
       <c r="H65" s="1">
         <v>6</v>
       </c>
@@ -1807,6 +1831,9 @@
       <c r="E66" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
       <c r="H66" s="1">
         <v>6</v>
       </c>
@@ -1821,6 +1848,9 @@
       <c r="C67" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
       <c r="H67" s="1">
         <v>6</v>
       </c>
@@ -1835,6 +1865,9 @@
       <c r="E68" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
       <c r="H68" s="1">
         <v>6</v>
       </c>
@@ -1852,6 +1885,9 @@
       <c r="F69" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
       <c r="H69" s="1">
         <v>6</v>
       </c>
@@ -1866,6 +1902,9 @@
       <c r="E70" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
       <c r="H70" s="1">
         <v>6</v>
       </c>
@@ -1880,6 +1919,9 @@
       <c r="E71" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
       <c r="H71" s="1">
         <v>6</v>
       </c>
@@ -1897,6 +1939,9 @@
       <c r="E72" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="G72">
+        <v>3</v>
+      </c>
       <c r="H72" s="1">
         <v>6</v>
       </c>
@@ -1911,6 +1956,9 @@
       <c r="E73" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
       <c r="H73" s="1">
         <v>6</v>
       </c>
@@ -1925,6 +1973,9 @@
       <c r="E74" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="G74">
+        <v>3</v>
+      </c>
       <c r="H74" s="1">
         <v>6</v>
       </c>
@@ -1939,6 +1990,9 @@
       <c r="E75" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G75">
+        <v>3</v>
+      </c>
       <c r="H75" s="1">
         <v>6</v>
       </c>
@@ -1953,6 +2007,9 @@
       <c r="E76" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="G76">
+        <v>3</v>
+      </c>
       <c r="H76" s="1">
         <v>6</v>
       </c>
@@ -1970,6 +2027,9 @@
       <c r="E77" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="G77">
+        <v>4</v>
+      </c>
       <c r="H77" s="1">
         <v>6</v>
       </c>
@@ -1987,6 +2047,9 @@
       <c r="F78" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="G78">
+        <v>4</v>
+      </c>
       <c r="H78" s="1">
         <v>6</v>
       </c>
@@ -2001,6 +2064,9 @@
       <c r="E79" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
       <c r="H79" s="1">
         <v>6</v>
       </c>
@@ -2015,6 +2081,9 @@
       <c r="E80" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="G80">
+        <v>4</v>
+      </c>
       <c r="H80" s="1">
         <v>6</v>
       </c>
@@ -2032,6 +2101,9 @@
       <c r="E81" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="G81">
+        <v>4</v>
+      </c>
       <c r="H81" s="1">
         <v>6</v>
       </c>
@@ -2046,6 +2118,9 @@
       <c r="E82" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
       <c r="H82" s="1">
         <v>6</v>
       </c>
@@ -2060,6 +2135,9 @@
       <c r="E83" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="G83">
+        <v>4</v>
+      </c>
       <c r="H83" s="1">
         <v>6</v>
       </c>
@@ -2074,6 +2152,9 @@
       <c r="E84" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G84">
+        <v>5</v>
+      </c>
       <c r="H84" s="1">
         <v>6</v>
       </c>
@@ -2091,6 +2172,9 @@
       <c r="E85" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="G85">
+        <v>5</v>
+      </c>
       <c r="H85" s="1">
         <v>6</v>
       </c>
@@ -2098,6 +2182,12 @@
     <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>126</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>30</v>

</xml_diff>